<commit_message>
Updated the job seekers file
</commit_message>
<xml_diff>
--- a/face_dataset/data_randomizer/job_seekers_data.xlsx
+++ b/face_dataset/data_randomizer/job_seekers_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ziv79\Desktop\Programming\JobCupid\JobCupid\face_dataset\data_randomizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E56A45-7F9F-4ACD-8747-CC6FD1E9752E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6132A518-3CAC-4344-A206-BA02CDEC3F8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="85">
   <si>
     <t>Name</t>
   </si>
@@ -262,6 +262,24 @@
   </si>
   <si>
     <t>https://images.generated.photos/2pKH2EYlZT-ZQKZyw6U-_eblf3czJ0z7c8iz-exi_8g/rs:fit:256:256/Z3M6Ly9nZW5lcmF0/ZWQtcGhvdG9zL3Yz/XzA3OTg1NTguanBn.jpg</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Free_Text</t>
+  </si>
+  <si>
+    <t>{'Mitz Marak': 1}</t>
+  </si>
+  <si>
+    <t>{'Cafe Yehoshua': 3}</t>
+  </si>
+  <si>
+    <t>{'Hagadir': 3}</t>
+  </si>
+  <si>
+    <t>{'Mitz Marak': 4}</t>
   </si>
 </sst>
 </file>
@@ -306,10 +324,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -591,491 +610,570 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" customWidth="1"/>
-    <col min="2" max="2" width="35.109375" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" customWidth="1"/>
-    <col min="5" max="5" width="20.21875" customWidth="1"/>
-    <col min="6" max="6" width="22.21875" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="1" max="2" width="12.77734375" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" customWidth="1"/>
+    <col min="6" max="6" width="20.21875" customWidth="1"/>
+    <col min="7" max="7" width="22.21875" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>57</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2">
+        <v>35</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>30</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>26</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>31</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>32</v>
       </c>
-      <c r="G4">
+      <c r="G4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H4">
         <v>38</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>27</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>31</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>38</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>25</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>30</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>45</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>25</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>31</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8">
+        <v>32</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>28</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>33</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>33</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>25</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>30</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>42</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>28</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>33</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>38</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>27</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>30</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>41</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>27</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>33</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13">
+        <v>31</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>29</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>33</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>45</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>26</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>31</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15">
+        <v>31</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>29</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>32</v>
       </c>
-      <c r="G15">
+      <c r="G15" t="s">
+        <v>82</v>
+      </c>
+      <c r="H15">
         <v>36</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16">
+        <v>29</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>26</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>30</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17">
+        <v>34</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>26</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>30</v>
       </c>
-      <c r="G17">
+      <c r="G17" t="s">
+        <v>83</v>
+      </c>
+      <c r="H17">
         <v>41</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18">
+        <v>32</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>26</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>31</v>
       </c>
-      <c r="G18">
+      <c r="G18" t="s">
+        <v>84</v>
+      </c>
+      <c r="H18">
         <v>32</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19">
+        <v>26</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>27</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>31</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>26</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>33</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>37</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21">
+        <v>24</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>27</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>30</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>35</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{82BC4C6C-F539-4186-AD96-1C1B88B0E363}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{82BC4C6C-F539-4186-AD96-1C1B88B0E363}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>